<commit_message>
Chapter 2 : Cell References
</commit_message>
<xml_diff>
--- a/Spreadsheet/Introduction to Google Sheets/data/Food Ingredients.xlsx
+++ b/Spreadsheet/Introduction to Google Sheets/data/Food Ingredients.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="190" yWindow="550" windowWidth="18880" windowHeight="6740"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -38,91 +41,128 @@
   </si>
   <si>
     <t>Flour</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>TAX</t>
+  </si>
+  <si>
+    <t>Price With Tax</t>
+  </si>
+  <si>
+    <t>Total With Tax</t>
+  </si>
+  <si>
+    <t>Kcal/Weight</t>
+  </si>
+  <si>
+    <t>Rounded Kcal/Weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="dd/MM/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
+    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -312,105 +352,233 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="3" max="3" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5">
-        <v>121.0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>186.0</v>
-      </c>
-      <c r="D2" s="7">
-        <v>43121.0</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="B2" s="7">
+        <v>121</v>
+      </c>
+      <c r="C2" s="11">
+        <v>43121</v>
+      </c>
+      <c r="D2" s="5">
         <v>0.4</v>
       </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9">
+        <f>E2*D2</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="G2" s="10">
+        <f>D2*$B$7</f>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="H2" s="10">
+        <f>E2*G2</f>
+        <v>0.252</v>
+      </c>
+      <c r="I2">
+        <v>323</v>
+      </c>
+      <c r="J2" s="9">
+        <f>I2/B2</f>
+        <v>2.669421487603306</v>
+      </c>
+      <c r="K2" s="9">
+        <f>ROUND(J2,2)</f>
+        <v>2.67</v>
+      </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
-        <v>125.0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>484.0</v>
-      </c>
-      <c r="D3" s="7">
-        <v>43831.0</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="B3" s="7">
+        <v>125</v>
+      </c>
+      <c r="C3" s="11">
+        <v>43831</v>
+      </c>
+      <c r="D3" s="5">
         <v>0.2</v>
       </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:F5" si="0">E3*D3</f>
+        <v>0.4</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G5" si="1">D3*$B$7</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" ref="H3:H5" si="2">E3*G3</f>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="I3">
+        <v>134</v>
+      </c>
+      <c r="J3" s="9">
+        <f t="shared" ref="J3:J5" si="3">I3/B3</f>
+        <v>1.0720000000000001</v>
+      </c>
+      <c r="K3" s="9">
+        <f t="shared" ref="K3:K5" si="4">ROUND(J3,2)</f>
+        <v>1.07</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5">
-        <v>65.0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>466.0</v>
-      </c>
-      <c r="D4" s="7">
-        <v>43120.0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>2.0</v>
+      <c r="B4" s="7">
+        <v>65</v>
+      </c>
+      <c r="C4" s="11">
+        <v>43120</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" si="1"/>
+        <v>0.42</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="2"/>
+        <v>1.26</v>
+      </c>
+      <c r="I4">
+        <v>243</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="3"/>
+        <v>3.7384615384615385</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="4"/>
+        <v>3.74</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
-        <v>190.0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>692.0</v>
-      </c>
-      <c r="D5" s="7">
-        <v>43344.0</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="B5" s="7">
+        <v>190</v>
+      </c>
+      <c r="C5" s="11">
+        <v>43344</v>
+      </c>
+      <c r="D5" s="5">
         <v>0.3</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3E-2</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="2"/>
+        <v>0.315</v>
+      </c>
+      <c r="I5">
+        <v>321</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="3"/>
+        <v>1.6894736842105262</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="4"/>
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>